<commit_message>
work update on 23/07/2020
</commit_message>
<xml_diff>
--- a/ReportsExcels/Joonk/JMR-rpt_DAILY_MANUFACTURE.xlsx
+++ b/ReportsExcels/Joonk/JMR-rpt_DAILY_MANUFACTURE.xlsx
@@ -365,6 +365,52 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -375,52 +421,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,19 +786,19 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22:H22"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" customWidth="1"/>
@@ -808,91 +808,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:13" ht="15.2" customHeight="1"/>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="18" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="19"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="17"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="24" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="19"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="19"/>
+      <c r="H5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="18"/>
       <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="19"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
@@ -907,24 +907,24 @@
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="19"/>
+      <c r="I6" s="18"/>
       <c r="J6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="19"/>
+      <c r="L6" s="18"/>
       <c r="M6" s="3" t="s">
         <v>12</v>
       </c>
@@ -951,17 +951,17 @@
       <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="16">
         <v>23.3</v>
       </c>
-      <c r="L7" s="19"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="5">
         <v>22.37</v>
       </c>
@@ -988,13 +988,13 @@
       <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="19"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="22">
-        <v>0</v>
-      </c>
-      <c r="L8" s="23"/>
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="21"/>
       <c r="M8" s="13">
         <v>0</v>
       </c>
@@ -1050,571 +1050,571 @@
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="19"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:13" ht="18" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="24" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="19"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="26" t="s">
+      <c r="A12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="27" t="s">
+      <c r="F12" s="18"/>
+      <c r="G12" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="26" t="s">
+      <c r="H12" s="18"/>
+      <c r="I12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="26" t="s">
+      <c r="J12" s="18"/>
+      <c r="K12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="19"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="28">
+      <c r="B13" s="18"/>
+      <c r="C13" s="23">
         <v>127777</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="28">
-        <v>0</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="31">
+      <c r="D13" s="18"/>
+      <c r="E13" s="23">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="25">
         <v>127777</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="28">
+      <c r="H13" s="18"/>
+      <c r="I13" s="23">
         <v>83830</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="28">
-        <v>0</v>
-      </c>
-      <c r="L13" s="19"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="23">
+        <v>0</v>
+      </c>
+      <c r="L13" s="18"/>
       <c r="M13" s="10">
         <v>83830</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="29">
+      <c r="B14" s="18"/>
+      <c r="C14" s="24">
         <v>4669</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="28">
-        <v>0</v>
-      </c>
-      <c r="F14" s="19"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="23">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18"/>
       <c r="G14" s="30">
         <v>4669</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="29">
+      <c r="H14" s="21"/>
+      <c r="I14" s="24">
         <v>2070</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="28">
-        <v>0</v>
-      </c>
-      <c r="L14" s="19"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="23">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18"/>
       <c r="M14" s="14">
         <v>2070</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="30">
         <v>123108</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="31">
-        <v>0</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="31">
+      <c r="D15" s="21"/>
+      <c r="E15" s="25">
+        <v>0</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="25">
         <v>123108</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="31">
+      <c r="H15" s="18"/>
+      <c r="I15" s="25">
         <v>81760</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="31">
-        <v>0</v>
-      </c>
-      <c r="L15" s="19"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="25">
+        <v>0</v>
+      </c>
+      <c r="L15" s="18"/>
       <c r="M15" s="10">
         <v>81760</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16" s="19"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="18"/>
+      <c r="K16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="18"/>
       <c r="M16" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="18" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="24" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="24" t="s">
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="24" t="s">
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="20"/>
-      <c r="M17" s="19"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="26" t="s">
+      <c r="A18" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="26" t="s">
+      <c r="D18" s="18"/>
+      <c r="E18" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="26" t="s">
+      <c r="F18" s="18"/>
+      <c r="G18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="26" t="s">
+      <c r="H18" s="18"/>
+      <c r="I18" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="26" t="s">
+      <c r="J18" s="18"/>
+      <c r="K18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="19"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="28">
+      <c r="B19" s="18"/>
+      <c r="C19" s="23">
         <v>5992</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="28">
+      <c r="D19" s="18"/>
+      <c r="E19" s="23">
         <v>571217</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="29">
+      <c r="F19" s="18"/>
+      <c r="G19" s="24">
         <v>11240</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="29">
+      <c r="H19" s="21"/>
+      <c r="I19" s="24">
         <v>677203</v>
       </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="28">
-        <v>0</v>
-      </c>
-      <c r="L19" s="19"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="23">
+        <v>0</v>
+      </c>
+      <c r="L19" s="18"/>
       <c r="M19" s="9">
         <v>0</v>
       </c>
-      <c r="N19" s="34" t="s">
+      <c r="N19" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="28">
-        <v>0</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="28">
-        <v>0</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="28">
-        <v>0</v>
-      </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="28">
-        <v>0</v>
-      </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="28">
-        <v>0</v>
-      </c>
-      <c r="L20" s="19"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="23">
+        <v>0</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="23">
+        <v>0</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="23">
+        <v>0</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="23">
+        <v>0</v>
+      </c>
+      <c r="J20" s="18"/>
+      <c r="K20" s="23">
+        <v>0</v>
+      </c>
+      <c r="L20" s="18"/>
       <c r="M20" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="31">
+      <c r="B21" s="18"/>
+      <c r="C21" s="25">
         <v>5992</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="31">
+      <c r="D21" s="18"/>
+      <c r="E21" s="25">
         <v>571217</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="31">
+      <c r="F21" s="18"/>
+      <c r="G21" s="25">
         <v>11240</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="31">
+      <c r="H21" s="18"/>
+      <c r="I21" s="25">
         <v>677203</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="31">
-        <v>0</v>
-      </c>
-      <c r="L21" s="19"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="25">
+        <v>0</v>
+      </c>
+      <c r="L21" s="18"/>
       <c r="M21" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="28">
+      <c r="B22" s="18"/>
+      <c r="C22" s="23">
         <v>1396</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="28">
+      <c r="D22" s="18"/>
+      <c r="E22" s="23">
         <v>127777</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="29">
+      <c r="F22" s="18"/>
+      <c r="G22" s="24">
         <v>3346</v>
       </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="29">
+      <c r="H22" s="21"/>
+      <c r="I22" s="24">
         <v>153095</v>
       </c>
-      <c r="J22" s="23"/>
-      <c r="K22" s="28">
-        <v>0</v>
-      </c>
-      <c r="L22" s="19"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="23">
+        <v>0</v>
+      </c>
+      <c r="L22" s="18"/>
       <c r="M22" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="28">
+      <c r="B23" s="18"/>
+      <c r="C23" s="23">
         <v>23.3</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="28">
+      <c r="D23" s="18"/>
+      <c r="E23" s="23">
         <v>22.37</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="29">
+      <c r="F23" s="18"/>
+      <c r="G23" s="24">
         <v>29.77</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="29">
+      <c r="H23" s="21"/>
+      <c r="I23" s="24">
         <v>22.61</v>
       </c>
-      <c r="J23" s="23"/>
-      <c r="K23" s="28">
-        <v>0</v>
-      </c>
-      <c r="L23" s="19"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="18"/>
       <c r="M23" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="28">
-        <v>0</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="28">
+      <c r="B24" s="18"/>
+      <c r="C24" s="23">
+        <v>0</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="23">
         <v>129881</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="28">
+      <c r="F24" s="18"/>
+      <c r="G24" s="23">
         <v>3250</v>
       </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="28">
+      <c r="H24" s="18"/>
+      <c r="I24" s="23">
         <v>154939</v>
       </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="28">
-        <v>0</v>
-      </c>
-      <c r="L24" s="19"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="23">
+        <v>0</v>
+      </c>
+      <c r="L24" s="18"/>
       <c r="M24" s="9">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="29">
-        <v>0</v>
-      </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="29">
+      <c r="B25" s="21"/>
+      <c r="C25" s="24">
+        <v>0</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="24">
         <v>71515</v>
       </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="29">
+      <c r="F25" s="21"/>
+      <c r="G25" s="24">
         <v>3250</v>
       </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="29">
+      <c r="H25" s="21"/>
+      <c r="I25" s="24">
         <v>151891</v>
       </c>
-      <c r="J25" s="23"/>
-      <c r="K25" s="28">
-        <v>0</v>
-      </c>
-      <c r="L25" s="19"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="23">
+        <v>0</v>
+      </c>
+      <c r="L25" s="18"/>
       <c r="M25" s="9">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="28">
-        <v>0</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="28">
-        <v>0</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="28">
-        <v>0</v>
-      </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="28">
-        <v>0</v>
-      </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="28">
-        <v>0</v>
-      </c>
-      <c r="L26" s="19"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="23">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="23">
+        <v>0</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="23">
+        <v>0</v>
+      </c>
+      <c r="H26" s="18"/>
+      <c r="I26" s="23">
+        <v>0</v>
+      </c>
+      <c r="J26" s="18"/>
+      <c r="K26" s="23">
+        <v>0</v>
+      </c>
+      <c r="L26" s="18"/>
       <c r="M26" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="28">
-        <v>0</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="28">
-        <v>0</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="28">
-        <v>0</v>
-      </c>
-      <c r="H27" s="19"/>
-      <c r="I27" s="28">
-        <v>0</v>
-      </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="28">
-        <v>0</v>
-      </c>
-      <c r="L27" s="19"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="23">
+        <v>0</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="23">
+        <v>0</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="23">
+        <v>0</v>
+      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="23">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18"/>
+      <c r="K27" s="23">
+        <v>0</v>
+      </c>
+      <c r="L27" s="18"/>
       <c r="M27" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="18" customHeight="1">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="21" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="21" t="s">
+      <c r="D28" s="18"/>
+      <c r="E28" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="21" t="s">
+      <c r="F28" s="18"/>
+      <c r="G28" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="21" t="s">
+      <c r="H28" s="18"/>
+      <c r="I28" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="L28" s="20"/>
-      <c r="M28" s="19"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:14" ht="18" customHeight="1">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="22" t="s">
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="23"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="21"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="24" t="s">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="24" t="s">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="19"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="2" t="s">
@@ -1784,6 +1784,116 @@
     <row r="36" spans="1:13" ht="7.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="127">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:M10"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="G29:M29"/>
     <mergeCell ref="B30:E30"/>
@@ -1801,116 +1911,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:M10"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="K8:L8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="1.3055598425196899" header="0.25" footer="0.25"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>